<commit_message>
changes in pom and apitestscenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata.xlsx
+++ b/src/test/resources/Testdata.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ariz.siddiqui\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\seleniumWD\parallel-universe\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0080E2C-F6BD-4B0E-92EC-584188BAB788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF84A711-5B29-4AD3-B49E-7A873BB9ECB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3558AE3D-7585-4784-972F-238043367F40}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3558AE3D-7585-4784-972F-238043367F40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Api" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>emailAddress</t>
   </si>
@@ -70,6 +71,24 @@
   </si>
   <si>
     <t>Jawad22</t>
+  </si>
+  <si>
+    <t>API Data01</t>
+  </si>
+  <si>
+    <t>ScenarioID</t>
+  </si>
+  <si>
+    <t>CompanyID</t>
+  </si>
+  <si>
+    <t>6044</t>
+  </si>
+  <si>
+    <t>6045</t>
+  </si>
+  <si>
+    <t>1739</t>
   </si>
 </sst>
 </file>
@@ -105,8 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F3A640-03BC-4378-B077-454C63967AC4}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,4 +510,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A6F562-33AF-4B68-8C1D-A5071A781D3B}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add constant and proper used of env variables of intellij
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata.xlsx
+++ b/src/test/resources/Testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\seleniumWD\parallel-universe\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E1E9AD-318C-4CF7-B24E-A50EEDD628EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425CFF5D-1726-471D-866D-23820CA412C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{3558AE3D-7585-4784-972F-238043367F40}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>emailAddress</t>
   </si>
@@ -76,22 +76,25 @@
     <t>API Data01</t>
   </si>
   <si>
+    <t>1739</t>
+  </si>
+  <si>
+    <t>API Data02</t>
+  </si>
+  <si>
+    <t>ScenarioID</t>
+  </si>
+  <si>
+    <t>CompanyID</t>
+  </si>
+  <si>
+    <t>6046</t>
+  </si>
+  <si>
     <t>6044</t>
   </si>
   <si>
     <t>6045</t>
-  </si>
-  <si>
-    <t>1739</t>
-  </si>
-  <si>
-    <t>API Data02</t>
-  </si>
-  <si>
-    <t>ScenarioID</t>
-  </si>
-  <si>
-    <t>CompanyID</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,11 +520,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A6F562-33AF-4B68-8C1D-A5071A781D3B}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -534,10 +535,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -545,21 +546,32 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reformatting of code, added test in web,moved excel filepath inside env variable
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata.xlsx
+++ b/src/test/resources/Testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\seleniumWD\parallel-universe\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425CFF5D-1726-471D-866D-23820CA412C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8470B795-6A93-44DB-896C-89572DEE866B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{3558AE3D-7585-4784-972F-238043367F40}"/>
   </bookViews>
@@ -76,9 +76,6 @@
     <t>API Data01</t>
   </si>
   <si>
-    <t>1739</t>
-  </si>
-  <si>
     <t>API Data02</t>
   </si>
   <si>
@@ -88,13 +85,16 @@
     <t>CompanyID</t>
   </si>
   <si>
-    <t>6046</t>
-  </si>
-  <si>
-    <t>6044</t>
-  </si>
-  <si>
-    <t>6045</t>
+    <t>127</t>
+  </si>
+  <si>
+    <t>285</t>
+  </si>
+  <si>
+    <t>286</t>
+  </si>
+  <si>
+    <t>287</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A6F562-33AF-4B68-8C1D-A5071A781D3B}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -535,10 +537,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -546,21 +548,21 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -568,10 +570,10 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>